<commit_message>
fixed for shop pugin
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Shop.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Shop.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -18,19 +13,11 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159">
   <si>
     <t>Id</t>
   </si>
@@ -56,6 +43,9 @@
     <t>Level</t>
   </si>
   <si>
+    <t>Count</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -77,6 +67,9 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Upload</t>
+  </si>
+  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -501,17 +494,19 @@
   </si>
   <si>
     <t>18</t>
-  </si>
-  <si>
-    <t>Upload</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -526,12 +521,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +691,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -677,20 +1004,262 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="0.399945066682943"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="0.399945066682943"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="0.399945066682943"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -738,13 +1307,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -758,20 +1375,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
     <tableStyle name="MySqlDefault" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1098,31 +1707,32 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="9" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10:I71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.1769911504425" customWidth="1"/>
+    <col min="2" max="2" width="8.17699115044248" customWidth="1"/>
+    <col min="3" max="3" width="28.1769911504425" customWidth="1"/>
+    <col min="4" max="4" width="21.4513274336283" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6371681415929" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1147,36 +1757,42 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:9">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:9">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="8" t="b">
         <v>0</v>
@@ -1199,10 +1815,13 @@
       <c r="H3" s="8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:9">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="8" t="b">
         <v>0</v>
@@ -1225,10 +1844,13 @@
       <c r="H4" s="8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:9">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="8" t="b">
         <v>1</v>
@@ -1251,10 +1873,13 @@
       <c r="H5" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:9">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8" t="b">
         <v>0</v>
@@ -1277,10 +1902,13 @@
       <c r="H6" s="8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:9">
       <c r="A7" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -1303,10 +1931,13 @@
       <c r="H7" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:9">
       <c r="A8" s="9" t="s">
-        <v>157</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1329,10 +1960,13 @@
       <c r="H8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="4" customFormat="1" ht="14.25" spans="1:8">
       <c r="A9" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1342,18 +1976,18 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1367,19 +2001,22 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -1393,19 +2030,22 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1419,19 +2059,22 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1445,19 +2088,22 @@
       <c r="H13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1471,19 +2117,22 @@
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1497,19 +2146,22 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1523,19 +2175,22 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1549,19 +2204,22 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1575,19 +2233,22 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1601,19 +2262,22 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1627,19 +2291,22 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1653,19 +2320,22 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1679,19 +2349,22 @@
       <c r="H22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1705,19 +2378,22 @@
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1731,19 +2407,22 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1757,19 +2436,22 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1783,19 +2465,22 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1809,19 +2494,22 @@
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1835,19 +2523,22 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1861,19 +2552,22 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1887,19 +2581,22 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1913,19 +2610,22 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1939,19 +2639,22 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1965,19 +2668,22 @@
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1991,19 +2697,22 @@
       <c r="H34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -2017,19 +2726,22 @@
       <c r="H35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -2043,19 +2755,22 @@
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2069,19 +2784,22 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2095,19 +2813,22 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B39">
         <v>5</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2121,19 +2842,22 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2147,19 +2871,22 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B41">
         <v>5</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2173,19 +2900,22 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B42">
         <v>5</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2199,19 +2929,22 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2225,19 +2958,22 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44">
         <v>6</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2251,19 +2987,22 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B45">
         <v>6</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2277,19 +3016,22 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B46">
         <v>6</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2303,19 +3045,22 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B47">
         <v>6</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2329,19 +3074,22 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B48">
         <v>6</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2355,19 +3103,22 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49">
         <v>6</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2381,19 +3132,22 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B50">
         <v>6</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2407,19 +3161,22 @@
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B51">
         <v>6</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2433,19 +3190,22 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B52">
         <v>6</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -2459,19 +3219,22 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B53">
         <v>6</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2485,19 +3248,22 @@
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B54">
         <v>6</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2511,19 +3277,22 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B55">
         <v>7</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2537,19 +3306,22 @@
       <c r="H55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B56">
         <v>8</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2563,19 +3335,22 @@
       <c r="H56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B57">
         <v>9</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2589,19 +3364,22 @@
       <c r="H57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B58">
         <v>10</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2615,19 +3393,22 @@
       <c r="H58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B59">
         <v>11</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -2641,19 +3422,22 @@
       <c r="H59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B60">
         <v>12</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -2667,19 +3451,22 @@
       <c r="H60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B61">
         <v>13</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -2693,19 +3480,22 @@
       <c r="H61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B62">
         <v>14</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2719,19 +3509,22 @@
       <c r="H62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B63">
         <v>15</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2745,19 +3538,22 @@
       <c r="H63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B64">
         <v>16</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -2771,19 +3567,22 @@
       <c r="H64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B65">
         <v>17</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2797,19 +3596,22 @@
       <c r="H65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B66">
         <v>18</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2823,19 +3625,22 @@
       <c r="H66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B67">
         <v>19</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2849,19 +3654,22 @@
       <c r="H67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B68">
         <v>20</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2875,19 +3683,22 @@
       <c r="H68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B69">
         <v>21</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2901,19 +3712,22 @@
       <c r="H69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="12" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B70">
         <v>22</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2927,19 +3741,22 @@
       <c r="H70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B71">
         <v>23</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2953,16 +3770,18 @@
       <c r="H71">
         <v>0</v>
       </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I8 J7:J8 B7:H8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>